<commit_message>
[task] Create Rate Monotonic Analysis 	- Add printing of timings to Floor and Elevatos subsystems 	- Change placement of timings files 	- Create rate monotonic analysis Excel file
</commit_message>
<xml_diff>
--- a/Documentation/Rate Monotonic Analysis.xlsx
+++ b/Documentation/Rate Monotonic Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brams\eclipse-workspace\ElevatorControlSystem\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2F17D0-6FFF-4C66-A510-4C912A8FAACA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A10472F-FDE7-454D-BD9C-9C00C9648EF2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C4736C0A-3F15-4FCE-AE55-4B9BEE0C69D5}"/>
+    <workbookView xWindow="-10230" yWindow="3615" windowWidth="21600" windowHeight="11385" xr2:uid="{C4736C0A-3F15-4FCE-AE55-4B9BEE0C69D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>Process Name</t>
   </si>
@@ -88,13 +88,31 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Sporadic</t>
+  </si>
+  <si>
+    <t>Without Sporadic Events (Sorted By Periods - Lowest To Highest)</t>
+  </si>
+  <si>
+    <t>With Sporadic Events (Sorted By Periods, Sporadic Events Sorted By Execution Times  - Lowest To Highest)</t>
+  </si>
+  <si>
+    <t>Regular Events</t>
+  </si>
+  <si>
+    <t>Sporadic Events</t>
+  </si>
+  <si>
+    <t>Events Not Currently Used</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,13 +120,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -120,13 +174,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -439,129 +502,351 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5772EAC1-8E4A-4C7E-BB37-DF308B99676F}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="42" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="12" max="12" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>1692365399.453552</v>
+      </c>
+      <c r="C3">
+        <v>1156930709.2391305</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1692365399.453552</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1156930709.2391305</v>
+      </c>
+      <c r="J3" s="1">
+        <v>7</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>1701653388.4615386</v>
+      </c>
+      <c r="C4">
+        <v>355579485.79234976</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1701653388.4615386</v>
+      </c>
+      <c r="I4" s="1">
+        <v>355579485.79234976</v>
+      </c>
+      <c r="J4" s="1">
+        <v>6</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2047697266</v>
+      </c>
+      <c r="C5">
+        <v>1672788.0794701986</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="1">
+        <v>2047697266</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1672788.0794701986</v>
+      </c>
+      <c r="J5" s="1">
+        <v>5</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>6177664031.5789471</v>
+      </c>
+      <c r="C6">
+        <v>1741127575</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="1">
+        <v>6177664031.5789471</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1741127575</v>
+      </c>
+      <c r="J6" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>7385023046.1538458</v>
+      </c>
+      <c r="C7">
+        <v>409642.85714285716</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="1">
+        <v>7385023046.1538458</v>
+      </c>
+      <c r="I7" s="1">
+        <v>409642.85714285716</v>
+      </c>
+      <c r="J7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>7925038963.1578951</v>
+      </c>
+      <c r="C8">
+        <v>606092.30769230775</v>
+      </c>
+      <c r="D8">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="1">
+        <v>7925038963.1578951</v>
+      </c>
+      <c r="I8" s="1">
+        <v>606092.30769230775</v>
+      </c>
+      <c r="J8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>48006942400</v>
+      </c>
+      <c r="C9">
+        <v>883300</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="1">
+        <v>48006942400</v>
+      </c>
+      <c r="I9" s="1">
+        <v>883300</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="2">
+        <v>600</v>
+      </c>
+      <c r="J11" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="2">
+        <v>95900</v>
+      </c>
+      <c r="J12" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="2">
+        <v>779200</v>
+      </c>
+      <c r="J13" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="2">
+        <v>4361700</v>
+      </c>
+      <c r="J14" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>2293961061.3636365</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>5999635789.4736843</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="J15" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G18" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="H18" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="I18" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>7547320820</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>47998155100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
+      <c r="J18" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H8:H22">
+    <sortCondition ref="H8"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[task] Highlight non-Scheduler events in the Rate Monotonic Analysis 	- Non-scheduler events are now red 	- Rate Monotonic analysis only includes Scheduler events
</commit_message>
<xml_diff>
--- a/Documentation/Rate Monotonic Analysis.xlsx
+++ b/Documentation/Rate Monotonic Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brams\eclipse-workspace\ElevatorControlSystem\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA31468-A0BC-41F8-A104-BC8D29B4C532}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEBEC63-F8C6-4404-BDBD-A3450BE84F69}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C4736C0A-3F15-4FCE-AE55-4B9BEE0C69D5}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
   <si>
     <t>Process Name</t>
   </si>
@@ -121,13 +121,16 @@
   </si>
   <si>
     <t>CPU Utilization</t>
+  </si>
+  <si>
+    <t>Non-Scheduler Events (i.e Floor and Elevator Events)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,8 +159,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,8 +190,13 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -188,21 +204,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5772EAC1-8E4A-4C7E-BB37-DF308B99676F}">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,7 +568,7 @@
     <col min="9" max="9" width="21" customWidth="1"/>
     <col min="10" max="10" width="14.85546875" customWidth="1"/>
     <col min="12" max="12" width="10.7109375" customWidth="1"/>
-    <col min="13" max="13" width="29.28515625" customWidth="1"/>
+    <col min="13" max="13" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -588,44 +622,44 @@
         <v>1615893401.5625</v>
       </c>
       <c r="D3">
-        <f>K3</f>
+        <f t="shared" ref="D3:D8" si="0">K3</f>
         <v>6</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="3">
         <v>1880939657.5916231</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="3">
         <v>1615893401.5625</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="3">
         <f>I3 / H3</f>
         <v>0.85908837906661428</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="3">
         <v>6</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
-        <f t="shared" ref="A4:A8" si="0">G4</f>
+        <f t="shared" ref="A4:A8" si="1">G4</f>
         <v>FLOOR_SENSOR_MODE</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B9" si="1">H4</f>
+        <f t="shared" ref="B4:B8" si="2">H4</f>
         <v>1897162159.375</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C8" si="2">I4</f>
+        <f t="shared" ref="C4:C8" si="3">I4</f>
         <v>1738588.0932642487</v>
       </c>
       <c r="D4">
-        <f>K4</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -638,7 +672,7 @@
         <v>1738588.0932642487</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" ref="J4:J18" si="3">I4 / H4</f>
+        <f t="shared" ref="J4:J8" si="4">I4 / H4</f>
         <v>9.1641512280479396E-4</v>
       </c>
       <c r="K4" s="1">
@@ -648,58 +682,58 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
+        <f t="shared" si="1"/>
+        <v>ELEVATOR_DIRECTION_MODE</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="2"/>
+        <v>1907110071.7277486</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="3"/>
+        <v>42206079.203125</v>
+      </c>
+      <c r="D5">
         <f t="shared" si="0"/>
-        <v>ELEVATOR_DIRECTION_MODE</v>
-      </c>
-      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1907110071.7277486</v>
+      </c>
+      <c r="I5" s="3">
+        <v>42206079.203125</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="4"/>
+        <v>2.2130908870345564E-2</v>
+      </c>
+      <c r="K5" s="3">
+        <v>4</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
         <f t="shared" si="1"/>
-        <v>1907110071.7277486</v>
-      </c>
-      <c r="C5">
+        <v>FLOOR_REQUEST_MODE</v>
+      </c>
+      <c r="B6">
         <f t="shared" si="2"/>
-        <v>42206079.203125</v>
-      </c>
-      <c r="D5">
-        <f>K5</f>
-        <v>4</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1907110071.7277486</v>
-      </c>
-      <c r="I5" s="1">
-        <v>42206079.203125</v>
-      </c>
-      <c r="J5" s="1">
+        <v>6000050536.8421049</v>
+      </c>
+      <c r="C6">
         <f t="shared" si="3"/>
-        <v>2.2130908870345564E-2</v>
-      </c>
-      <c r="K5" s="1">
-        <v>4</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="str">
+        <v>1471479.8</v>
+      </c>
+      <c r="D6">
         <f t="shared" si="0"/>
-        <v>FLOOR_REQUEST_MODE</v>
-      </c>
-      <c r="B6">
-        <f t="shared" si="1"/>
-        <v>6000050536.8421049</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="2"/>
-        <v>1471479.8</v>
-      </c>
-      <c r="D6">
-        <f>K6</f>
         <v>3</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -712,62 +746,65 @@
         <v>1471479.8</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.4524456768566766E-4</v>
       </c>
       <c r="K6" s="1">
         <v>3</v>
       </c>
+      <c r="M6" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
+        <f t="shared" si="1"/>
+        <v>SEND_DESTINATION_TO_ELEVATOR_MODE</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="2"/>
+        <v>6027394553.1578951</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="3"/>
+        <v>2352538545.0999999</v>
+      </c>
+      <c r="D7">
         <f t="shared" si="0"/>
-        <v>SEND_DESTINATION_TO_ELEVATOR_MODE</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="3">
         <v>6027394553.1578951</v>
       </c>
-      <c r="C7">
-        <f t="shared" si="2"/>
+      <c r="I7" s="3">
         <v>2352538545.0999999</v>
       </c>
-      <c r="D7">
-        <f>K7</f>
-        <v>2</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="1">
-        <v>6027394553.1578951</v>
-      </c>
-      <c r="I7" s="1">
-        <v>2352538545.0999999</v>
-      </c>
-      <c r="J7" s="1">
-        <f t="shared" si="3"/>
+      <c r="J7" s="3">
+        <f t="shared" si="4"/>
         <v>0.3903077066470535</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
+        <f t="shared" si="1"/>
+        <v>ERROR_MESSAGE_MODE</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="2"/>
+        <v>48000077010</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="3"/>
+        <v>2360200</v>
+      </c>
+      <c r="D8">
         <f t="shared" si="0"/>
-        <v>ERROR_MESSAGE_MODE</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="1"/>
-        <v>48000077010</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="2"/>
-        <v>2360200</v>
-      </c>
-      <c r="D8">
-        <f>K8</f>
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -780,7 +817,7 @@
         <v>2360200</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.9170754445004169E-5</v>
       </c>
       <c r="K8" s="1">
@@ -788,19 +825,19 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="3">
         <v>1901</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K10" s="2">
+      <c r="J10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="3">
         <v>11</v>
       </c>
       <c r="M10" t="s">
@@ -874,8 +911,8 @@
         <v>28</v>
       </c>
       <c r="N13">
-        <f>SUM(J3:J8)</f>
-        <v>1.2727378250289489</v>
+        <f>SUM(J4, J6, J8)</f>
+        <v>1.2108304449354658E-3</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -895,57 +932,59 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G16" s="3" t="s">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K16" s="3">
+      <c r="H16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G17" s="3" t="s">
+    <row r="17" spans="7:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K17" s="3">
+      <c r="H17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K17" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G18" s="3" t="s">
+    <row r="18" spans="7:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K18" s="3">
+      <c r="H18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K18" s="4">
         <v>0</v>
       </c>
     </row>
+    <row r="19" spans="7:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L11:L16">
     <sortCondition ref="L11"/>

</xml_diff>

<commit_message>
[task] Change error mode to sporadic event
</commit_message>
<xml_diff>
--- a/Documentation/Rate Monotonic Analysis.xlsx
+++ b/Documentation/Rate Monotonic Analysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brams\eclipse-workspace\ElevatorControlSystem\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEBEC63-F8C6-4404-BDBD-A3450BE84F69}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FAB0E01-23B7-4391-B430-C755DAA93455}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C4736C0A-3F15-4FCE-AE55-4B9BEE0C69D5}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>Process Name</t>
   </si>
@@ -551,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5772EAC1-8E4A-4C7E-BB37-DF308B99676F}">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +623,7 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D8" si="0">K3</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>7</v>
@@ -639,7 +639,7 @@
         <v>0.85908837906661428</v>
       </c>
       <c r="K3" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>22</v>
@@ -660,7 +660,7 @@
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>4</v>
@@ -676,7 +676,7 @@
         <v>9.1641512280479396E-4</v>
       </c>
       <c r="K4" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>23</v>
@@ -697,7 +697,7 @@
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>6</v>
@@ -713,7 +713,7 @@
         <v>2.2130908870345564E-2</v>
       </c>
       <c r="K5" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>24</v>
@@ -734,7 +734,7 @@
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>3</v>
@@ -750,7 +750,7 @@
         <v>2.4524456768566766E-4</v>
       </c>
       <c r="K6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>30</v>
@@ -771,7 +771,7 @@
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>8</v>
@@ -787,40 +787,6 @@
         <v>0.3903077066470535</v>
       </c>
       <c r="K7" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="str">
-        <f t="shared" si="1"/>
-        <v>ERROR_MESSAGE_MODE</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="2"/>
-        <v>48000077010</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="3"/>
-        <v>2360200</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="1">
-        <v>48000077010</v>
-      </c>
-      <c r="I8" s="1">
-        <v>2360200</v>
-      </c>
-      <c r="J8" s="1">
-        <f t="shared" si="4"/>
-        <v>4.9170754445004169E-5</v>
-      </c>
-      <c r="K8" s="1">
         <v>1</v>
       </c>
     </row>
@@ -864,7 +830,7 @@
         <v>27</v>
       </c>
       <c r="N11">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -888,18 +854,18 @@
       </c>
       <c r="N12">
         <f>N11 * (POWER(2, 1/N11) - 1)</f>
-        <v>0.7347722898562381</v>
+        <v>0.74349177498517549</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G13" s="2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I13" s="2">
-        <v>2694699</v>
+        <v>2360200</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>18</v>
@@ -911,19 +877,19 @@
         <v>28</v>
       </c>
       <c r="N13">
-        <f>SUM(J4, J6, J8)</f>
-        <v>1.2108304449354658E-3</v>
+        <f>SUM(J4, J6)</f>
+        <v>1.1616596904904617E-3</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G14" s="2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>18</v>
+      <c r="I14" s="2">
+        <v>2694699</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>18</v>
@@ -932,27 +898,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K16" s="4">
-        <v>0</v>
-      </c>
-    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="7:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G17" s="4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>18</v>
@@ -969,7 +935,7 @@
     </row>
     <row r="18" spans="7:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>18</v>
@@ -984,7 +950,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="7:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="7:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="7:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L11:L16">
     <sortCondition ref="L11"/>

</xml_diff>